<commit_message>
Fixed issue with upf_barcelona subj01 - now marked as session error fussy, per #57
</commit_message>
<xml_diff>
--- a/processed_data/participants_cleaned/UPF_Barcelona_participant_data.xlsx
+++ b/processed_data/participants_cleaned/UPF_Barcelona_participant_data.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5500" yWindow="980" windowWidth="29840" windowHeight="23300"/>
+    <workbookView xWindow="7080" yWindow="5200" windowWidth="29840" windowHeight="23300"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -899,7 +899,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -914,7 +914,7 @@
   <dimension ref="A1:BF968"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="A87" sqref="A68:XFD87"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1130,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>53</v>

</xml_diff>